<commit_message>
add code to view by tag
</commit_message>
<xml_diff>
--- a/src/api/Docs/populate.xlsx
+++ b/src/api/Docs/populate.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -40,31 +37,91 @@
     <t>author</t>
   </si>
   <si>
+    <t>Sean001</t>
+  </si>
+  <si>
+    <t>Team up</t>
+  </si>
+  <si>
+    <t>work, labor, team, recruits, helper, free_lancer, demo, shared, community</t>
+  </si>
+  <si>
+    <t>A website for free lancers to team up and get a project temporarily</t>
+  </si>
+  <si>
+    <t>Sean cheng</t>
+  </si>
+  <si>
+    <t>Sean002</t>
+  </si>
+  <si>
+    <t>Public account</t>
+  </si>
+  <si>
+    <t>Shared, managements, open_source, privacy,demo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similar to yopmail that you can use use for testing and for privacy. Or the fake phone number girls give to guys. </t>
+  </si>
+  <si>
     <t>Sean003</t>
   </si>
   <si>
-    <t>Team up</t>
-  </si>
-  <si>
-    <t>work, labor, team, recruits, helper, free_lancer, demo</t>
-  </si>
-  <si>
-    <t>A website for free lancers to team up and get a project temporarily</t>
-  </si>
-  <si>
-    <t>Sean cheng</t>
-  </si>
-  <si>
-    <t>Sean004</t>
-  </si>
-  <si>
-    <t>Public account</t>
-  </si>
-  <si>
-    <t>share, managements, open_source, privacy,demo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Similar to yopmail that you can use use for testing and for privacy. Or the fake phone number girls give to guys. </t>
+    <t>Dumbies</t>
+  </si>
+  <si>
+    <t>Dumb, Zombies, idiocracy, comedy, pun, sci-fi</t>
+  </si>
+  <si>
+    <t>Human become dumber and dumber, eventually becomes zombie like creature</t>
+  </si>
+  <si>
+    <t>sean004</t>
+  </si>
+  <si>
+    <t>Neighborhood breakfast group</t>
+  </si>
+  <si>
+    <t>Community, food, breakfast, shared, helper</t>
+  </si>
+  <si>
+    <t>To save time and add variety of the breakfast, set up a potluck like service</t>
+  </si>
+  <si>
+    <t>sean005</t>
+  </si>
+  <si>
+    <t>Cat-as-trophy</t>
+  </si>
+  <si>
+    <t>Catastrophe, pun, word, merch, trophy</t>
+  </si>
+  <si>
+    <t>A trophy for cat or bad events</t>
+  </si>
+  <si>
+    <t>sean006</t>
+  </si>
+  <si>
+    <t>Freelancer pipelines</t>
+  </si>
+  <si>
+    <t>free_lancer, work, labor, shared, outsource, pyramid</t>
+  </si>
+  <si>
+    <t>A network of freelancers, each person has queues, and can outsource down one level to other free lancer to hep digest the workload, with minimum commission (can only be passed down one level)</t>
+  </si>
+  <si>
+    <t>Sean007</t>
+  </si>
+  <si>
+    <t>Share knowledges</t>
+  </si>
+  <si>
+    <t>Handcraft, community, decentralized, skill, knowledge, movement</t>
+  </si>
+  <si>
+    <t>Each person in the group shares whatever knowledge they have with others, with a short sessions. For example, gold welding, jewelry making, plant, construction, fix car, solder, welding.</t>
   </si>
 </sst>
 </file>
@@ -74,7 +131,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -86,13 +143,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +173,12 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -231,56 +299,53 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -304,6 +369,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -320,10 +386,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -500,11 +566,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -513,34 +582,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -788,12 +857,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1084,7 +1153,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1365,11 +1434,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H11"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
@@ -1377,158 +1444,193 @@
     <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="14.7" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
+    <row r="2" ht="50.7" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="3">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="3">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s" s="3">
         <v>8</v>
       </c>
+      <c r="B2" t="s" s="4">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" t="s" s="7">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" ht="56.25" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s" s="5">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s" s="6">
-        <v>11</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" t="s" s="8">
+    <row r="3" ht="74.7" customHeight="1">
+      <c r="A3" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" t="s" s="12">
         <v>12</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" t="s" s="8">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" ht="80.05" customHeight="1">
-      <c r="A4" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" t="s" s="13">
+    <row r="4" ht="62.7" customHeight="1">
+      <c r="A4" t="s" s="8">
         <v>17</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" t="s" s="13">
-        <v>13</v>
+      <c r="B4" t="s" s="9">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" t="s" s="12">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
+    <row r="5" ht="50.7" customHeight="1">
+      <c r="A5" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="9">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" t="s" s="12">
+        <v>24</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" t="s" s="12">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+    <row r="6" ht="26.7" customHeight="1">
+      <c r="A6" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s" s="9">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" t="s" s="12">
+        <v>28</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" t="s" s="12">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
+    <row r="7" ht="146.7" customHeight="1">
+      <c r="A7" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s" s="10">
+        <v>31</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" t="s" s="12">
+        <v>32</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" t="s" s="12">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+    <row r="8" ht="134.7" customHeight="1">
+      <c r="A8" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" t="s" s="12">
+        <v>36</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" t="s" s="12">
+        <v>12</v>
+      </c>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
change _id to yyyymmddhhmmss + index for bulk
</commit_message>
<xml_diff>
--- a/src/api/Docs/populate.xlsx
+++ b/src/api/Docs/populate.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
-  <si>
-    <t>id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+  <si>
+    <t>author</t>
   </si>
   <si>
     <t>idea</t>
@@ -34,10 +34,7 @@
     <t>note</t>
   </si>
   <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>Sean001</t>
+    <t>Sean cheng</t>
   </si>
   <si>
     <t>Team up</t>
@@ -49,12 +46,6 @@
     <t>A website for free lancers to team up and get a project temporarily</t>
   </si>
   <si>
-    <t>Sean cheng</t>
-  </si>
-  <si>
-    <t>Sean002</t>
-  </si>
-  <si>
     <t>Public account</t>
   </si>
   <si>
@@ -64,9 +55,6 @@
     <t xml:space="preserve">Similar to yopmail that you can use use for testing and for privacy. Or the fake phone number girls give to guys. </t>
   </si>
   <si>
-    <t>Sean003</t>
-  </si>
-  <si>
     <t>Dumbies</t>
   </si>
   <si>
@@ -76,9 +64,6 @@
     <t>Human become dumber and dumber, eventually becomes zombie like creature</t>
   </si>
   <si>
-    <t>sean004</t>
-  </si>
-  <si>
     <t>Neighborhood breakfast group</t>
   </si>
   <si>
@@ -88,9 +73,6 @@
     <t>To save time and add variety of the breakfast, set up a potluck like service</t>
   </si>
   <si>
-    <t>sean005</t>
-  </si>
-  <si>
     <t>Cat-as-trophy</t>
   </si>
   <si>
@@ -100,9 +82,6 @@
     <t>A trophy for cat or bad events</t>
   </si>
   <si>
-    <t>sean006</t>
-  </si>
-  <si>
     <t>Freelancer pipelines</t>
   </si>
   <si>
@@ -110,9 +89,6 @@
   </si>
   <si>
     <t>A network of freelancers, each person has queues, and can outsource down one level to other free lancer to hep digest the workload, with minimum commission (can only be passed down one level)</t>
-  </si>
-  <si>
-    <t>Sean007</t>
   </si>
   <si>
     <t>Share knowledges</t>
@@ -299,7 +275,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -309,43 +285,34 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -368,8 +335,8 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1434,14 +1401,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="8" width="16.3516" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.7" customHeight="1">
@@ -1466,169 +1433,143 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" ht="50.7" customHeight="1">
       <c r="A2" t="s" s="3">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s" s="4">
         <v>8</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="C2" t="s" s="5">
         <v>9</v>
-      </c>
-      <c r="C2" t="s" s="5">
-        <v>10</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" t="s" s="7">
-        <v>11</v>
+      <c r="F2" t="s" s="3">
+        <v>10</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" t="s" s="7">
-        <v>12</v>
-      </c>
     </row>
     <row r="3" ht="74.7" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="A3" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" t="s" s="7">
         <v>13</v>
       </c>
-      <c r="B3" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" t="s" s="12">
-        <v>16</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" t="s" s="12">
-        <v>12</v>
-      </c>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" ht="62.7" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" t="s" s="12">
-        <v>20</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" t="s" s="12">
-        <v>12</v>
-      </c>
+      <c r="A4" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s" s="9">
+        <v>15</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" ht="50.7" customHeight="1">
-      <c r="A5" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s" s="10">
-        <v>23</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" t="s" s="12">
-        <v>24</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" t="s" s="12">
-        <v>12</v>
-      </c>
+      <c r="A5" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s" s="9">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" ht="26.7" customHeight="1">
-      <c r="A6" t="s" s="8">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s" s="9">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>27</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" t="s" s="12">
-        <v>28</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" t="s" s="12">
-        <v>12</v>
-      </c>
+      <c r="A6" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" ht="146.7" customHeight="1">
-      <c r="A7" t="s" s="8">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s" s="10">
-        <v>31</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" t="s" s="12">
-        <v>32</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" t="s" s="12">
-        <v>12</v>
-      </c>
+      <c r="A7" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s" s="9">
+        <v>24</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" ht="134.7" customHeight="1">
-      <c r="A8" t="s" s="8">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s" s="9">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" t="s" s="12">
-        <v>36</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" t="s" s="12">
-        <v>12</v>
-      </c>
+      <c r="A8" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" ht="14.7" customHeight="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>